<commit_message>
update test and pypanel library
</commit_message>
<xml_diff>
--- a/docs/PyPanel_class-subclass_listing.xlsx
+++ b/docs/PyPanel_class-subclass_listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Documents\GitHub\Robot_Friend_FeatherWing\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0653DA6-DE57-4AE9-A83A-7D145A7B4852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6E2E76-1C51-4786-B8B0-C8119EA72971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3285" yWindow="-15060" windowWidth="21960" windowHeight="14865" xr2:uid="{AC7C8F05-EBF5-45D4-A160-8BEF9604E9A4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="192">
   <si>
     <t>crickit</t>
   </si>
@@ -480,18 +480,12 @@
     <t>play_file</t>
   </si>
   <si>
-    <t>panel (via PyBadger)</t>
-  </si>
-  <si>
     <t>clear</t>
   </si>
   <si>
     <t>degrees</t>
   </si>
   <si>
-    <t>mode</t>
-  </si>
-  <si>
     <t>position</t>
   </si>
   <si>
@@ -501,12 +495,6 @@
     <t>reset</t>
   </si>
   <si>
-    <t>write</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
     <t>right</t>
   </si>
   <si>
@@ -567,24 +555,6 @@
     <t>dot</t>
   </si>
   <si>
-    <t>stamp</t>
-  </si>
-  <si>
-    <t>clearstamp</t>
-  </si>
-  <si>
-    <t>clearstamps</t>
-  </si>
-  <si>
-    <t>undo</t>
-  </si>
-  <si>
-    <t>speed</t>
-  </si>
-  <si>
-    <t>towards</t>
-  </si>
-  <si>
     <t>xcor</t>
   </si>
   <si>
@@ -594,9 +564,6 @@
     <t>heading</t>
   </si>
   <si>
-    <t>distance</t>
-  </si>
-  <si>
     <t>pendown</t>
   </si>
   <si>
@@ -615,124 +582,34 @@
     <t>pencolor</t>
   </si>
   <si>
-    <t>fillcolor</t>
-  </si>
-  <si>
-    <t>filling</t>
-  </si>
-  <si>
-    <t>begin_fill</t>
-  </si>
-  <si>
-    <t>end_fill</t>
-  </si>
-  <si>
-    <t>showturtle</t>
-  </si>
-  <si>
     <t>st</t>
   </si>
   <si>
-    <t>hideturtle</t>
-  </si>
-  <si>
     <t>ht</t>
   </si>
   <si>
-    <t>isvisible</t>
-  </si>
-  <si>
-    <t>shape</t>
-  </si>
-  <si>
-    <t>resizemode</t>
-  </si>
-  <si>
-    <t>shapesize</t>
-  </si>
-  <si>
     <t>turtlesize</t>
   </si>
   <si>
-    <t>sheerfactor</t>
-  </si>
-  <si>
-    <t>settiltangle</t>
-  </si>
-  <si>
-    <t>tiltangle</t>
-  </si>
-  <si>
-    <t>shapetransform</t>
-  </si>
-  <si>
-    <t>get_shapepoly</t>
-  </si>
-  <si>
-    <t>onclick</t>
-  </si>
-  <si>
-    <t>onrelease</t>
-  </si>
-  <si>
-    <t>ondrag</t>
-  </si>
-  <si>
-    <t>begin_poly</t>
-  </si>
-  <si>
-    <t>end_poly</t>
-  </si>
-  <si>
-    <t>get_poly</t>
-  </si>
-  <si>
-    <t>clone</t>
-  </si>
-  <si>
-    <t>getturtle</t>
-  </si>
-  <si>
     <t>getpen</t>
   </si>
   <si>
-    <t>getscreen</t>
-  </si>
-  <si>
-    <t>setundobuffer</t>
-  </si>
-  <si>
-    <t>undobufferentries</t>
-  </si>
-  <si>
-    <t>colormode</t>
-  </si>
-  <si>
-    <t>getcanvas</t>
-  </si>
-  <si>
-    <t>getshapes</t>
-  </si>
-  <si>
-    <t>register_shape</t>
-  </si>
-  <si>
     <t>addshape</t>
   </si>
   <si>
-    <t>window_height</t>
-  </si>
-  <si>
-    <t>window_width</t>
-  </si>
-  <si>
     <t>penup</t>
   </si>
   <si>
     <t>FourWire</t>
   </si>
   <si>
-    <t>joystick (PyBadge only)</t>
+    <t>back</t>
+  </si>
+  <si>
+    <t>panel</t>
+  </si>
+  <si>
+    <t>joystick (PyGamer only)</t>
   </si>
 </sst>
 </file>
@@ -825,12 +702,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DA466E5A-04BD-4507-8777-CE8FDE78B869}" name="Table5" displayName="Table5" ref="C3:L91" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="C3:L91" xr:uid="{9123DC94-EE13-4BE4-B3EE-2E51DDED7A9A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DA466E5A-04BD-4507-8777-CE8FDE78B869}" name="Table5" displayName="Table5" ref="C3:L52" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="C3:L52" xr:uid="{9123DC94-EE13-4BE4-B3EE-2E51DDED7A9A}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4F5AC77C-371A-4B88-9B87-F34963FFDAD9}" name="board"/>
     <tableColumn id="2" xr3:uid="{84F888BF-DDAB-48F6-918B-8EF49FF838E0}" name="i2c"/>
-    <tableColumn id="3" xr3:uid="{1247F7E4-BD50-4D6D-BE7C-C82492802170}" name="panel (via PyBadger)"/>
+    <tableColumn id="3" xr3:uid="{1247F7E4-BD50-4D6D-BE7C-C82492802170}" name="panel"/>
     <tableColumn id="4" xr3:uid="{DFAB215F-B715-430A-B3DE-FCDFEEE369C4}" name="display"/>
     <tableColumn id="5" xr3:uid="{5CEE48B7-F5AF-4168-9C4E-D120D68D59EE}" name="crickit"/>
     <tableColumn id="6" xr3:uid="{4F0CB020-2851-4450-A8CA-C48F8A209D40}" name="terminalio"/>
@@ -1143,10 +1020,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L91"/>
+  <dimension ref="B1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1054,7 @@
         <v>106</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>107</v>
@@ -1227,7 +1104,7 @@
         <v>89</v>
       </c>
       <c r="K4" t="s">
-        <v>227</v>
+        <v>186</v>
       </c>
       <c r="L4" t="s">
         <v>111</v>
@@ -1259,7 +1136,7 @@
         <v>90</v>
       </c>
       <c r="K5" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="L5" t="s">
         <v>110</v>
@@ -1285,7 +1162,7 @@
         <v>91</v>
       </c>
       <c r="K6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="L6" t="s">
         <v>109</v>
@@ -1308,10 +1185,10 @@
         <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="K7" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -1334,7 +1211,7 @@
         <v>92</v>
       </c>
       <c r="K8" t="s">
-        <v>214</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -1357,7 +1234,7 @@
         <v>93</v>
       </c>
       <c r="K9" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -1377,7 +1254,7 @@
         <v>94</v>
       </c>
       <c r="K10" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -1397,7 +1274,7 @@
         <v>95</v>
       </c>
       <c r="K11" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -1414,7 +1291,7 @@
         <v>98</v>
       </c>
       <c r="K12" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -1431,7 +1308,7 @@
         <v>96</v>
       </c>
       <c r="K13" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
@@ -1448,7 +1325,7 @@
         <v>97</v>
       </c>
       <c r="K14" t="s">
-        <v>217</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -1462,7 +1339,7 @@
         <v>29</v>
       </c>
       <c r="K15" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -1476,7 +1353,7 @@
         <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>223</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
@@ -1484,13 +1361,13 @@
         <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>232</v>
+        <v>191</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K17" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
@@ -1504,7 +1381,7 @@
         <v>32</v>
       </c>
       <c r="K18" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
@@ -1518,7 +1395,7 @@
         <v>24</v>
       </c>
       <c r="K19" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
@@ -1532,7 +1409,7 @@
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
@@ -1546,7 +1423,7 @@
         <v>37</v>
       </c>
       <c r="K21" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
@@ -1560,7 +1437,7 @@
         <v>2</v>
       </c>
       <c r="K22" t="s">
-        <v>215</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
@@ -1571,10 +1448,10 @@
         <v>139</v>
       </c>
       <c r="G23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K23" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
@@ -1588,7 +1465,7 @@
         <v>3</v>
       </c>
       <c r="K24" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
@@ -1602,7 +1479,7 @@
         <v>12</v>
       </c>
       <c r="K25" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
@@ -1616,7 +1493,7 @@
         <v>13</v>
       </c>
       <c r="K26" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
@@ -1630,7 +1507,7 @@
         <v>14</v>
       </c>
       <c r="K27" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
@@ -1641,7 +1518,7 @@
         <v>15</v>
       </c>
       <c r="K28" t="s">
-        <v>210</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.25">
@@ -1652,7 +1529,7 @@
         <v>4</v>
       </c>
       <c r="K29" t="s">
-        <v>224</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
@@ -1663,7 +1540,7 @@
         <v>5</v>
       </c>
       <c r="K30" t="s">
-        <v>219</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.25">
@@ -1674,7 +1551,7 @@
         <v>6</v>
       </c>
       <c r="K31" t="s">
-        <v>220</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
@@ -1685,7 +1562,7 @@
         <v>7</v>
       </c>
       <c r="K32" t="s">
-        <v>225</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
@@ -1696,7 +1573,7 @@
         <v>8</v>
       </c>
       <c r="K33" t="s">
-        <v>218</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
@@ -1707,7 +1584,7 @@
         <v>9</v>
       </c>
       <c r="K34" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
@@ -1718,7 +1595,7 @@
         <v>10</v>
       </c>
       <c r="K35" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
@@ -1729,7 +1606,7 @@
         <v>11</v>
       </c>
       <c r="K36" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
@@ -1740,7 +1617,7 @@
         <v>22</v>
       </c>
       <c r="K37" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
@@ -1751,7 +1628,7 @@
         <v>33</v>
       </c>
       <c r="K38" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
@@ -1762,7 +1639,7 @@
         <v>34</v>
       </c>
       <c r="K39" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
@@ -1773,7 +1650,7 @@
         <v>35</v>
       </c>
       <c r="K40" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
@@ -1784,7 +1661,7 @@
         <v>36</v>
       </c>
       <c r="K41" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
@@ -1792,7 +1669,7 @@
         <v>77</v>
       </c>
       <c r="K42" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.25">
@@ -1800,7 +1677,7 @@
         <v>78</v>
       </c>
       <c r="K43" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.25">
@@ -1808,274 +1685,56 @@
         <v>79</v>
       </c>
       <c r="K44" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>80</v>
       </c>
-      <c r="K45" t="s">
-        <v>213</v>
-      </c>
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>81</v>
       </c>
-      <c r="K46" t="s">
-        <v>212</v>
-      </c>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>82</v>
       </c>
-      <c r="K47" t="s">
-        <v>188</v>
-      </c>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>83</v>
       </c>
-      <c r="K48" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>84</v>
       </c>
-      <c r="K49" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>85</v>
       </c>
-      <c r="K50" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>86</v>
       </c>
-      <c r="K51" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>87</v>
-      </c>
-      <c r="K52" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K53" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K54" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K55" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K56" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K57" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K58" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K59" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K60" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K61" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K62" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K63" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K64" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K65" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K66" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K67" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K68" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K69" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K70" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K71" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="72" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K72" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="73" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K73" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="74" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K74" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="75" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K75" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="76" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K76" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="77" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K77" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="78" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K78" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="79" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K79" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="80" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K80" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="81" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K81" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="82" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K82" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="83" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K83" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="84" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K84" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="85" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K85" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="86" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K86" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="87" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K87" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="88" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K88" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="89" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K89" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="90" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K90" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="91" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K91" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L4:L6">
     <sortCondition ref="L4:L6"/>
   </sortState>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
-  <pageSetup scale="73" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="69" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;D  &amp;T&amp;C&amp;F&amp;A&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>